<commit_message>
Prototype code done, need to add comments
</commit_message>
<xml_diff>
--- a/familyview_project/data/fyp_dataset.xlsx
+++ b/familyview_project/data/fyp_dataset.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\w1891238_fyp\familyview_project\familyview_project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D1BA0-A6C8-4E82-9E14-063359B0D7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="137">
   <si>
     <t>Title</t>
   </si>
@@ -217,9 +226,6 @@
     <t>My Neighbour Totoro</t>
   </si>
   <si>
-    <t xml:space="preserve">Animation </t>
-  </si>
-  <si>
     <t>Dead Poets Society</t>
   </si>
   <si>
@@ -371,9 +377,6 @@
   </si>
   <si>
     <t>Iron Man</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action </t>
   </si>
   <si>
     <t>Avatar</t>
@@ -433,15 +436,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -452,36 +456,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -671,25 +683,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D414"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection sqref="A1:D414"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.25"/>
-    <col customWidth="1" min="2" max="2" width="21.75"/>
-    <col customWidth="1" min="3" max="3" width="16.75"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,13 +728,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="D2" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -725,13 +742,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>1957.0</v>
+        <v>1957</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -739,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="D4" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -753,13 +770,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="D5" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -767,13 +784,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>1994.0</v>
+        <v>1994</v>
       </c>
       <c r="D6" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -781,13 +798,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="D7" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -795,13 +812,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D8" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -809,13 +826,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="1">
-        <v>1980.0</v>
+        <v>1980</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -823,13 +840,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="D10" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -837,13 +854,13 @@
         <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>1946.0</v>
+        <v>1946</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -851,13 +868,13 @@
         <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>1997.0</v>
+        <v>1997</v>
       </c>
       <c r="D12" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -865,13 +882,13 @@
         <v>16</v>
       </c>
       <c r="C13" s="1">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -879,13 +896,13 @@
         <v>16</v>
       </c>
       <c r="C14" s="1">
-        <v>1985.0</v>
+        <v>1985</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -893,13 +910,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -907,13 +924,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1">
-        <v>1994.0</v>
+        <v>1994</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -921,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="D17" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -935,13 +952,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -949,13 +966,13 @@
         <v>20</v>
       </c>
       <c r="C19" s="1">
-        <v>1942.0</v>
+        <v>1942</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -963,13 +980,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -977,13 +994,13 @@
         <v>16</v>
       </c>
       <c r="C21" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="D21" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -991,13 +1008,13 @@
         <v>25</v>
       </c>
       <c r="C22" s="1">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1005,13 +1022,13 @@
         <v>10</v>
       </c>
       <c r="C23" s="1">
-        <v>1981.0</v>
+        <v>1981</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1019,13 +1036,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="D24" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1033,13 +1050,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1047,13 +1064,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="D26" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1061,13 +1078,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1075,13 +1092,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="1">
-        <v>1995.0</v>
+        <v>1995</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1089,13 +1106,13 @@
         <v>5</v>
       </c>
       <c r="C29" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="D29" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1103,13 +1120,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1117,13 +1134,13 @@
         <v>42</v>
       </c>
       <c r="C31" s="1">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="D31" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
@@ -1131,13 +1148,13 @@
         <v>44</v>
       </c>
       <c r="C32" s="1">
-        <v>1952.0</v>
+        <v>1952</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1145,13 +1162,13 @@
         <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1159,13 +1176,13 @@
         <v>16</v>
       </c>
       <c r="C34" s="1">
-        <v>1983.0</v>
+        <v>1983</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1173,13 +1190,13 @@
         <v>16</v>
       </c>
       <c r="C35" s="1">
-        <v>1968.0</v>
+        <v>1968</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -1187,13 +1204,13 @@
         <v>49</v>
       </c>
       <c r="C36" s="1">
-        <v>1941.0</v>
+        <v>1941</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1201,13 +1218,13 @@
         <v>25</v>
       </c>
       <c r="C37" s="1">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -1215,13 +1232,13 @@
         <v>10</v>
       </c>
       <c r="C38" s="1">
-        <v>1989.0</v>
+        <v>1989</v>
       </c>
       <c r="D38" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>52</v>
       </c>
@@ -1229,13 +1246,13 @@
         <v>44</v>
       </c>
       <c r="C39" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D39" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
@@ -1243,13 +1260,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="1">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="D40" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
@@ -1257,13 +1274,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="D41" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
@@ -1271,13 +1288,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="1">
-        <v>1998.0</v>
+        <v>1998</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>56</v>
       </c>
@@ -1285,13 +1302,13 @@
         <v>16</v>
       </c>
       <c r="C43" s="1">
-        <v>1993.0</v>
+        <v>1993</v>
       </c>
       <c r="D43" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -1299,13 +1316,13 @@
         <v>58</v>
       </c>
       <c r="C44" s="1">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="D44" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
@@ -1313,13 +1330,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="D45" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>60</v>
       </c>
@@ -1327,13 +1344,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="1">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -1341,13 +1358,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="1">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
@@ -1355,13 +1372,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -1369,13 +1386,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="1">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -1383,13 +1400,13 @@
         <v>7</v>
       </c>
       <c r="C50" s="1">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="D50" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
@@ -1397,13 +1414,13 @@
         <v>10</v>
       </c>
       <c r="C51" s="1">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="D51" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -1411,965 +1428,2730 @@
         <v>5</v>
       </c>
       <c r="C52" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="D52" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="1">
-        <v>1989.0</v>
+        <v>1989</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="1">
-        <v>2007.0</v>
+        <v>2007</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C57" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="1">
-        <v>1975.0</v>
+        <v>1975</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D59" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="1">
-        <v>2019.0</v>
-      </c>
-      <c r="D59" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1976</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1976.0</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C61" s="1">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="D61" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C62" s="1">
-        <v>1939.0</v>
+        <v>1939</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="1">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C64" s="1">
-        <v>1965.0</v>
+        <v>1965</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C65" s="1">
-        <v>1993.0</v>
+        <v>1993</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D66" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C67" s="1">
-        <v>1992.0</v>
+        <v>1992</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C68" s="1">
-        <v>1991.0</v>
+        <v>1991</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="D69" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C70" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D70" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="1">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="D71" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C72" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="D72" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C73" s="1">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="D73" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="1">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="D74" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C75" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="1">
-        <v>2025.0</v>
+        <v>2025</v>
       </c>
       <c r="D76" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C78" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="D79" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2024</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C80" s="1">
-        <v>2024.0</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C82" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="D82" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="D83" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C84" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="D85" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="1">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="1">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C88" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D89" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="1">
-        <v>2001.0</v>
-      </c>
-      <c r="D89" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D90" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C90" s="1">
-        <v>2018.0</v>
-      </c>
-      <c r="D90" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D91" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" s="1">
-        <v>2016.0</v>
-      </c>
-      <c r="D91" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C92" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="1">
-        <v>1989.0</v>
+        <v>1989</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C95" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C96" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="D96" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C97" s="1">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C98" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D98" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="99">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C99" s="1">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C100" s="1">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="D100" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C101" s="1">
-        <v>1997.0</v>
+        <v>1997</v>
       </c>
       <c r="D101" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D102" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C102" s="1">
-        <v>2008.0</v>
-      </c>
-      <c r="D102" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C103" s="1">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="D103" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C104" s="1">
-        <v>1982.0</v>
+        <v>1982</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="D105" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="106">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C106" s="1">
-        <v>1984.0</v>
+        <v>1984</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C107" s="1">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="D107" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="108">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C108" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="D109" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C110" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="1">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="D111" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C112" s="1">
-        <v>2003.0</v>
+        <v>2003</v>
       </c>
       <c r="D112" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C113" s="1">
-        <v>2008.0</v>
+        <v>2008</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C114" s="1">
-        <v>2010.0</v>
+        <v>2010</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C115" s="1">
-        <v>1973.0</v>
+        <v>1973</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C116" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="D116" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="117">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C117" s="1">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C118" s="1">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C119" s="1">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C120" s="1">
-        <v>1997.0</v>
+        <v>1997</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="2"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="2"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="2"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="2"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="2"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+    </row>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="2"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="2"/>
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="2"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="2"/>
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="2"/>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+    </row>
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="2"/>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+    </row>
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="2"/>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+    </row>
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="2"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+    </row>
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+    </row>
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="2"/>
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+    </row>
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="2"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+    </row>
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="2"/>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
+    </row>
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
+    </row>
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="2"/>
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+    </row>
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="2"/>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+    </row>
+    <row r="177" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="2"/>
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
+    </row>
+    <row r="178" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="2"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="2"/>
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="2"/>
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="2"/>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="2"/>
+      <c r="B183" s="2"/>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="2"/>
+      <c r="B184" s="2"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="2"/>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="2"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="2"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="2"/>
+      <c r="B188" s="2"/>
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="2"/>
+      <c r="B189" s="2"/>
+      <c r="C189" s="2"/>
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="2"/>
+      <c r="B190" s="2"/>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2"/>
+    </row>
+    <row r="191" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="2"/>
+      <c r="B191" s="2"/>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2"/>
+    </row>
+    <row r="192" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="2"/>
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
+    </row>
+    <row r="193" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="2"/>
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="2"/>
+      <c r="B194" s="2"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
+    </row>
+    <row r="195" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="2"/>
+      <c r="B195" s="2"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+    </row>
+    <row r="196" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="2"/>
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
+    </row>
+    <row r="197" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="2"/>
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
+    </row>
+    <row r="198" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="2"/>
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="2"/>
+      <c r="B199" s="2"/>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
+    </row>
+    <row r="200" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="2"/>
+      <c r="B200" s="2"/>
+      <c r="C200" s="2"/>
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="2"/>
+      <c r="B201" s="2"/>
+      <c r="C201" s="2"/>
+      <c r="D201" s="2"/>
+    </row>
+    <row r="202" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="2"/>
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
+    </row>
+    <row r="203" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="2"/>
+      <c r="B203" s="2"/>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
+    </row>
+    <row r="204" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="2"/>
+      <c r="B204" s="2"/>
+      <c r="C204" s="2"/>
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="2"/>
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+    </row>
+    <row r="206" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="2"/>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+    </row>
+    <row r="207" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="2"/>
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
+    </row>
+    <row r="208" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="2"/>
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
+    </row>
+    <row r="209" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="2"/>
+      <c r="B209" s="2"/>
+      <c r="C209" s="2"/>
+      <c r="D209" s="2"/>
+    </row>
+    <row r="210" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="2"/>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
+    </row>
+    <row r="211" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+    </row>
+    <row r="212" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="2"/>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+    </row>
+    <row r="213" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="2"/>
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+    </row>
+    <row r="214" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="2"/>
+      <c r="B214" s="2"/>
+      <c r="C214" s="2"/>
+      <c r="D214" s="2"/>
+    </row>
+    <row r="215" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="2"/>
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
+    </row>
+    <row r="216" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="2"/>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+    </row>
+    <row r="217" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="2"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+    </row>
+    <row r="218" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="2"/>
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+      <c r="D218" s="2"/>
+    </row>
+    <row r="219" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="2"/>
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="2"/>
+    </row>
+    <row r="220" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="2"/>
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
+    </row>
+    <row r="221" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="2"/>
+      <c r="B221" s="2"/>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
+    </row>
+    <row r="222" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="2"/>
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
+      <c r="D222" s="2"/>
+    </row>
+    <row r="223" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="2"/>
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
+    </row>
+    <row r="224" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="2"/>
+      <c r="B224" s="2"/>
+      <c r="C224" s="2"/>
+      <c r="D224" s="2"/>
+    </row>
+    <row r="225" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="2"/>
+      <c r="B225" s="2"/>
+      <c r="C225" s="2"/>
+      <c r="D225" s="2"/>
+    </row>
+    <row r="226" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="2"/>
+      <c r="B226" s="2"/>
+      <c r="C226" s="2"/>
+      <c r="D226" s="2"/>
+    </row>
+    <row r="227" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="2"/>
+      <c r="B227" s="2"/>
+      <c r="C227" s="2"/>
+      <c r="D227" s="2"/>
+    </row>
+    <row r="228" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="2"/>
+      <c r="B228" s="2"/>
+      <c r="C228" s="2"/>
+      <c r="D228" s="2"/>
+    </row>
+    <row r="229" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="2"/>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+    </row>
+    <row r="230" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="2"/>
+      <c r="B230" s="2"/>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2"/>
+    </row>
+    <row r="231" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="2"/>
+      <c r="B231" s="2"/>
+      <c r="C231" s="2"/>
+      <c r="D231" s="2"/>
+    </row>
+    <row r="232" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="2"/>
+      <c r="B232" s="2"/>
+      <c r="C232" s="2"/>
+      <c r="D232" s="2"/>
+    </row>
+    <row r="233" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="2"/>
+      <c r="B233" s="2"/>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+    </row>
+    <row r="234" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+    </row>
+    <row r="235" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="2"/>
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
+      <c r="D235" s="2"/>
+    </row>
+    <row r="236" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="2"/>
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+    </row>
+    <row r="237" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="2"/>
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+    </row>
+    <row r="238" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="2"/>
+      <c r="B238" s="2"/>
+      <c r="C238" s="2"/>
+      <c r="D238" s="2"/>
+    </row>
+    <row r="239" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="2"/>
+      <c r="B239" s="2"/>
+      <c r="C239" s="2"/>
+      <c r="D239" s="2"/>
+    </row>
+    <row r="240" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="2"/>
+      <c r="B240" s="2"/>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
+    </row>
+    <row r="241" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="2"/>
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+    </row>
+    <row r="242" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="2"/>
+      <c r="B242" s="2"/>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
+    </row>
+    <row r="243" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="2"/>
+      <c r="B243" s="2"/>
+      <c r="C243" s="2"/>
+      <c r="D243" s="2"/>
+    </row>
+    <row r="244" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="2"/>
+      <c r="B244" s="2"/>
+      <c r="C244" s="2"/>
+      <c r="D244" s="2"/>
+    </row>
+    <row r="245" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="2"/>
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
+      <c r="D245" s="2"/>
+    </row>
+    <row r="246" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="2"/>
+      <c r="B246" s="2"/>
+      <c r="C246" s="2"/>
+      <c r="D246" s="2"/>
+    </row>
+    <row r="247" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="2"/>
+      <c r="B247" s="2"/>
+      <c r="C247" s="2"/>
+      <c r="D247" s="2"/>
+    </row>
+    <row r="248" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="2"/>
+      <c r="B248" s="2"/>
+      <c r="C248" s="2"/>
+      <c r="D248" s="2"/>
+    </row>
+    <row r="249" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="2"/>
+      <c r="B249" s="2"/>
+      <c r="C249" s="2"/>
+      <c r="D249" s="2"/>
+    </row>
+    <row r="250" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="2"/>
+      <c r="B250" s="2"/>
+      <c r="C250" s="2"/>
+      <c r="D250" s="2"/>
+    </row>
+    <row r="251" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="2"/>
+      <c r="B251" s="2"/>
+      <c r="C251" s="2"/>
+      <c r="D251" s="2"/>
+    </row>
+    <row r="252" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="2"/>
+      <c r="B252" s="2"/>
+      <c r="C252" s="2"/>
+      <c r="D252" s="2"/>
+    </row>
+    <row r="253" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="2"/>
+      <c r="B253" s="2"/>
+      <c r="C253" s="2"/>
+      <c r="D253" s="2"/>
+    </row>
+    <row r="254" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="2"/>
+      <c r="B254" s="2"/>
+      <c r="C254" s="2"/>
+      <c r="D254" s="2"/>
+    </row>
+    <row r="255" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="2"/>
+      <c r="B255" s="2"/>
+      <c r="C255" s="2"/>
+      <c r="D255" s="2"/>
+    </row>
+    <row r="256" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="2"/>
+      <c r="B256" s="2"/>
+      <c r="C256" s="2"/>
+      <c r="D256" s="2"/>
+    </row>
+    <row r="257" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="2"/>
+      <c r="B257" s="2"/>
+      <c r="C257" s="2"/>
+      <c r="D257" s="2"/>
+    </row>
+    <row r="258" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="2"/>
+      <c r="B258" s="2"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+    </row>
+    <row r="259" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="2"/>
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+    </row>
+    <row r="260" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="2"/>
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
+      <c r="D260" s="2"/>
+    </row>
+    <row r="261" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="2"/>
+      <c r="B261" s="2"/>
+      <c r="C261" s="2"/>
+      <c r="D261" s="2"/>
+    </row>
+    <row r="262" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="2"/>
+      <c r="B262" s="2"/>
+      <c r="C262" s="2"/>
+      <c r="D262" s="2"/>
+    </row>
+    <row r="263" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="2"/>
+      <c r="B263" s="2"/>
+      <c r="C263" s="2"/>
+      <c r="D263" s="2"/>
+    </row>
+    <row r="264" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A264" s="2"/>
+      <c r="B264" s="2"/>
+      <c r="C264" s="2"/>
+      <c r="D264" s="2"/>
+    </row>
+    <row r="265" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="2"/>
+      <c r="B265" s="2"/>
+      <c r="C265" s="2"/>
+      <c r="D265" s="2"/>
+    </row>
+    <row r="266" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="2"/>
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+    </row>
+    <row r="267" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="2"/>
+      <c r="B267" s="2"/>
+      <c r="C267" s="2"/>
+      <c r="D267" s="2"/>
+    </row>
+    <row r="268" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="2"/>
+      <c r="B268" s="2"/>
+      <c r="C268" s="2"/>
+      <c r="D268" s="2"/>
+    </row>
+    <row r="269" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A269" s="2"/>
+      <c r="B269" s="2"/>
+      <c r="C269" s="2"/>
+      <c r="D269" s="2"/>
+    </row>
+    <row r="270" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="2"/>
+      <c r="B270" s="2"/>
+      <c r="C270" s="2"/>
+      <c r="D270" s="2"/>
+    </row>
+    <row r="271" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="2"/>
+      <c r="B271" s="2"/>
+      <c r="C271" s="2"/>
+      <c r="D271" s="2"/>
+    </row>
+    <row r="272" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="2"/>
+      <c r="B272" s="2"/>
+      <c r="C272" s="2"/>
+      <c r="D272" s="2"/>
+    </row>
+    <row r="273" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="2"/>
+      <c r="B273" s="2"/>
+      <c r="C273" s="2"/>
+      <c r="D273" s="2"/>
+    </row>
+    <row r="274" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="2"/>
+      <c r="B274" s="2"/>
+      <c r="C274" s="2"/>
+      <c r="D274" s="2"/>
+    </row>
+    <row r="275" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="2"/>
+      <c r="B275" s="2"/>
+      <c r="C275" s="2"/>
+      <c r="D275" s="2"/>
+    </row>
+    <row r="276" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="2"/>
+      <c r="B276" s="2"/>
+      <c r="C276" s="2"/>
+      <c r="D276" s="2"/>
+    </row>
+    <row r="277" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="2"/>
+      <c r="B277" s="2"/>
+      <c r="C277" s="2"/>
+      <c r="D277" s="2"/>
+    </row>
+    <row r="278" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="2"/>
+      <c r="B278" s="2"/>
+      <c r="C278" s="2"/>
+      <c r="D278" s="2"/>
+    </row>
+    <row r="279" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="2"/>
+      <c r="B279" s="2"/>
+      <c r="C279" s="2"/>
+      <c r="D279" s="2"/>
+    </row>
+    <row r="280" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="2"/>
+      <c r="B280" s="2"/>
+      <c r="C280" s="2"/>
+      <c r="D280" s="2"/>
+    </row>
+    <row r="281" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="2"/>
+      <c r="B281" s="2"/>
+      <c r="C281" s="2"/>
+      <c r="D281" s="2"/>
+    </row>
+    <row r="282" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="2"/>
+      <c r="B282" s="2"/>
+      <c r="C282" s="2"/>
+      <c r="D282" s="2"/>
+    </row>
+    <row r="283" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="2"/>
+      <c r="B283" s="2"/>
+      <c r="C283" s="2"/>
+      <c r="D283" s="2"/>
+    </row>
+    <row r="284" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="2"/>
+      <c r="B284" s="2"/>
+      <c r="C284" s="2"/>
+      <c r="D284" s="2"/>
+    </row>
+    <row r="285" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="2"/>
+      <c r="B285" s="2"/>
+      <c r="C285" s="2"/>
+      <c r="D285" s="2"/>
+    </row>
+    <row r="286" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="2"/>
+      <c r="B286" s="2"/>
+      <c r="C286" s="2"/>
+      <c r="D286" s="2"/>
+    </row>
+    <row r="287" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="2"/>
+      <c r="B287" s="2"/>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
+    </row>
+    <row r="288" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A288" s="2"/>
+      <c r="B288" s="2"/>
+      <c r="C288" s="2"/>
+      <c r="D288" s="2"/>
+    </row>
+    <row r="289" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="2"/>
+      <c r="B289" s="2"/>
+      <c r="C289" s="2"/>
+      <c r="D289" s="2"/>
+    </row>
+    <row r="290" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="2"/>
+      <c r="B290" s="2"/>
+      <c r="C290" s="2"/>
+      <c r="D290" s="2"/>
+    </row>
+    <row r="291" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="2"/>
+      <c r="B291" s="2"/>
+      <c r="C291" s="2"/>
+      <c r="D291" s="2"/>
+    </row>
+    <row r="292" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="2"/>
+      <c r="B292" s="2"/>
+      <c r="C292" s="2"/>
+      <c r="D292" s="2"/>
+    </row>
+    <row r="293" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A293" s="2"/>
+      <c r="B293" s="2"/>
+      <c r="C293" s="2"/>
+      <c r="D293" s="2"/>
+    </row>
+    <row r="294" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A294" s="2"/>
+      <c r="B294" s="2"/>
+      <c r="C294" s="2"/>
+      <c r="D294" s="2"/>
+    </row>
+    <row r="295" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="2"/>
+      <c r="B295" s="2"/>
+      <c r="C295" s="2"/>
+      <c r="D295" s="2"/>
+    </row>
+    <row r="296" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="2"/>
+      <c r="B296" s="2"/>
+      <c r="C296" s="2"/>
+      <c r="D296" s="2"/>
+    </row>
+    <row r="297" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="2"/>
+      <c r="B297" s="2"/>
+      <c r="C297" s="2"/>
+      <c r="D297" s="2"/>
+    </row>
+    <row r="298" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="2"/>
+      <c r="B298" s="2"/>
+      <c r="C298" s="2"/>
+      <c r="D298" s="2"/>
+    </row>
+    <row r="299" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="2"/>
+      <c r="B299" s="2"/>
+      <c r="C299" s="2"/>
+      <c r="D299" s="2"/>
+    </row>
+    <row r="300" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A300" s="2"/>
+      <c r="B300" s="2"/>
+      <c r="C300" s="2"/>
+      <c r="D300" s="2"/>
+    </row>
+    <row r="301" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A301" s="2"/>
+      <c r="B301" s="2"/>
+      <c r="C301" s="2"/>
+      <c r="D301" s="2"/>
+    </row>
+    <row r="302" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="2"/>
+      <c r="B302" s="2"/>
+      <c r="C302" s="2"/>
+      <c r="D302" s="2"/>
+    </row>
+    <row r="303" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="2"/>
+      <c r="B303" s="2"/>
+      <c r="C303" s="2"/>
+      <c r="D303" s="2"/>
+    </row>
+    <row r="304" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="2"/>
+      <c r="B304" s="2"/>
+      <c r="C304" s="2"/>
+      <c r="D304" s="2"/>
+    </row>
+    <row r="305" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="2"/>
+      <c r="B305" s="2"/>
+      <c r="C305" s="2"/>
+      <c r="D305" s="2"/>
+    </row>
+    <row r="306" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="2"/>
+      <c r="B306" s="2"/>
+      <c r="C306" s="2"/>
+      <c r="D306" s="2"/>
+    </row>
+    <row r="307" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="2"/>
+      <c r="B307" s="2"/>
+      <c r="C307" s="2"/>
+      <c r="D307" s="2"/>
+    </row>
+    <row r="308" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="2"/>
+      <c r="B308" s="2"/>
+      <c r="C308" s="2"/>
+      <c r="D308" s="2"/>
+    </row>
+    <row r="309" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="2"/>
+      <c r="B309" s="2"/>
+      <c r="C309" s="2"/>
+      <c r="D309" s="2"/>
+    </row>
+    <row r="310" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="2"/>
+      <c r="B310" s="2"/>
+      <c r="C310" s="2"/>
+      <c r="D310" s="2"/>
+    </row>
+    <row r="311" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="2"/>
+      <c r="B311" s="2"/>
+      <c r="C311" s="2"/>
+      <c r="D311" s="2"/>
+    </row>
+    <row r="312" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A312" s="2"/>
+      <c r="B312" s="2"/>
+      <c r="C312" s="2"/>
+      <c r="D312" s="2"/>
+    </row>
+    <row r="313" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="2"/>
+      <c r="B313" s="2"/>
+      <c r="C313" s="2"/>
+      <c r="D313" s="2"/>
+    </row>
+    <row r="314" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="2"/>
+      <c r="B314" s="2"/>
+      <c r="C314" s="2"/>
+      <c r="D314" s="2"/>
+    </row>
+    <row r="315" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A315" s="2"/>
+      <c r="B315" s="2"/>
+      <c r="C315" s="2"/>
+      <c r="D315" s="2"/>
+    </row>
+    <row r="316" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="2"/>
+      <c r="B316" s="2"/>
+      <c r="C316" s="2"/>
+      <c r="D316" s="2"/>
+    </row>
+    <row r="317" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A317" s="2"/>
+      <c r="B317" s="2"/>
+      <c r="C317" s="2"/>
+      <c r="D317" s="2"/>
+    </row>
+    <row r="318" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="2"/>
+      <c r="B318" s="2"/>
+      <c r="C318" s="2"/>
+      <c r="D318" s="2"/>
+    </row>
+    <row r="319" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="2"/>
+      <c r="B319" s="2"/>
+      <c r="C319" s="2"/>
+      <c r="D319" s="2"/>
+    </row>
+    <row r="320" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="2"/>
+      <c r="B320" s="2"/>
+      <c r="C320" s="2"/>
+      <c r="D320" s="2"/>
+    </row>
+    <row r="321" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="2"/>
+      <c r="B321" s="2"/>
+      <c r="C321" s="2"/>
+      <c r="D321" s="2"/>
+    </row>
+    <row r="322" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="2"/>
+      <c r="B322" s="2"/>
+      <c r="C322" s="2"/>
+      <c r="D322" s="2"/>
+    </row>
+    <row r="323" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="2"/>
+      <c r="B323" s="2"/>
+      <c r="C323" s="2"/>
+      <c r="D323" s="2"/>
+    </row>
+    <row r="324" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="2"/>
+      <c r="B324" s="2"/>
+      <c r="C324" s="2"/>
+      <c r="D324" s="2"/>
+    </row>
+    <row r="325" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="2"/>
+      <c r="B325" s="2"/>
+      <c r="C325" s="2"/>
+      <c r="D325" s="2"/>
+    </row>
+    <row r="326" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="2"/>
+      <c r="B326" s="2"/>
+      <c r="C326" s="2"/>
+      <c r="D326" s="2"/>
+    </row>
+    <row r="327" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="2"/>
+      <c r="B327" s="2"/>
+      <c r="C327" s="2"/>
+      <c r="D327" s="2"/>
+    </row>
+    <row r="328" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="2"/>
+      <c r="B328" s="2"/>
+      <c r="C328" s="2"/>
+      <c r="D328" s="2"/>
+    </row>
+    <row r="329" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="2"/>
+      <c r="B329" s="2"/>
+      <c r="C329" s="2"/>
+      <c r="D329" s="2"/>
+    </row>
+    <row r="330" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="2"/>
+      <c r="B330" s="2"/>
+      <c r="C330" s="2"/>
+      <c r="D330" s="2"/>
+    </row>
+    <row r="331" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="2"/>
+      <c r="B331" s="2"/>
+      <c r="C331" s="2"/>
+      <c r="D331" s="2"/>
+    </row>
+    <row r="332" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A332" s="2"/>
+      <c r="B332" s="2"/>
+      <c r="C332" s="2"/>
+      <c r="D332" s="2"/>
+    </row>
+    <row r="333" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A333" s="2"/>
+      <c r="B333" s="2"/>
+      <c r="C333" s="2"/>
+      <c r="D333" s="2"/>
+    </row>
+    <row r="334" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A334" s="2"/>
+      <c r="B334" s="2"/>
+      <c r="C334" s="2"/>
+      <c r="D334" s="2"/>
+    </row>
+    <row r="335" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A335" s="2"/>
+      <c r="B335" s="2"/>
+      <c r="C335" s="2"/>
+      <c r="D335" s="2"/>
+    </row>
+    <row r="336" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="2"/>
+      <c r="B336" s="2"/>
+      <c r="C336" s="2"/>
+      <c r="D336" s="2"/>
+    </row>
+    <row r="337" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A337" s="2"/>
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+      <c r="D337" s="2"/>
+    </row>
+    <row r="338" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="2"/>
+      <c r="B338" s="2"/>
+      <c r="C338" s="2"/>
+      <c r="D338" s="2"/>
+    </row>
+    <row r="339" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A339" s="2"/>
+      <c r="B339" s="2"/>
+      <c r="C339" s="2"/>
+      <c r="D339" s="2"/>
+    </row>
+    <row r="340" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="2"/>
+      <c r="B340" s="2"/>
+      <c r="C340" s="2"/>
+      <c r="D340" s="2"/>
+    </row>
+    <row r="341" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A341" s="2"/>
+      <c r="B341" s="2"/>
+      <c r="C341" s="2"/>
+      <c r="D341" s="2"/>
+    </row>
+    <row r="342" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A342" s="2"/>
+      <c r="B342" s="2"/>
+      <c r="C342" s="2"/>
+      <c r="D342" s="2"/>
+    </row>
+    <row r="343" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A343" s="2"/>
+      <c r="B343" s="2"/>
+      <c r="C343" s="2"/>
+      <c r="D343" s="2"/>
+    </row>
+    <row r="344" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="2"/>
+      <c r="B344" s="2"/>
+      <c r="C344" s="2"/>
+      <c r="D344" s="2"/>
+    </row>
+    <row r="345" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="2"/>
+      <c r="B345" s="2"/>
+      <c r="C345" s="2"/>
+      <c r="D345" s="2"/>
+    </row>
+    <row r="346" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="2"/>
+      <c r="B346" s="2"/>
+      <c r="C346" s="2"/>
+      <c r="D346" s="2"/>
+    </row>
+    <row r="347" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A347" s="2"/>
+      <c r="B347" s="2"/>
+      <c r="C347" s="2"/>
+      <c r="D347" s="2"/>
+    </row>
+    <row r="348" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A348" s="2"/>
+      <c r="B348" s="2"/>
+      <c r="C348" s="2"/>
+      <c r="D348" s="2"/>
+    </row>
+    <row r="349" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A349" s="2"/>
+      <c r="B349" s="2"/>
+      <c r="C349" s="2"/>
+      <c r="D349" s="2"/>
+    </row>
+    <row r="350" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="2"/>
+      <c r="B350" s="2"/>
+      <c r="C350" s="2"/>
+      <c r="D350" s="2"/>
+    </row>
+    <row r="351" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="2"/>
+      <c r="B351" s="2"/>
+      <c r="C351" s="2"/>
+      <c r="D351" s="2"/>
+    </row>
+    <row r="352" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="2"/>
+      <c r="B352" s="2"/>
+      <c r="C352" s="2"/>
+      <c r="D352" s="2"/>
+    </row>
+    <row r="353" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="2"/>
+      <c r="B353" s="2"/>
+      <c r="C353" s="2"/>
+      <c r="D353" s="2"/>
+    </row>
+    <row r="354" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="2"/>
+      <c r="B354" s="2"/>
+      <c r="C354" s="2"/>
+      <c r="D354" s="2"/>
+    </row>
+    <row r="355" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="2"/>
+      <c r="B355" s="2"/>
+      <c r="C355" s="2"/>
+      <c r="D355" s="2"/>
+    </row>
+    <row r="356" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="2"/>
+      <c r="B356" s="2"/>
+      <c r="C356" s="2"/>
+      <c r="D356" s="2"/>
+    </row>
+    <row r="357" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="2"/>
+      <c r="B357" s="2"/>
+      <c r="C357" s="2"/>
+      <c r="D357" s="2"/>
+    </row>
+    <row r="358" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="2"/>
+      <c r="B358" s="2"/>
+      <c r="C358" s="2"/>
+      <c r="D358" s="2"/>
+    </row>
+    <row r="359" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="2"/>
+      <c r="B359" s="2"/>
+      <c r="C359" s="2"/>
+      <c r="D359" s="2"/>
+    </row>
+    <row r="360" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="2"/>
+      <c r="B360" s="2"/>
+      <c r="C360" s="2"/>
+      <c r="D360" s="2"/>
+    </row>
+    <row r="361" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="2"/>
+      <c r="B361" s="2"/>
+      <c r="C361" s="2"/>
+      <c r="D361" s="2"/>
+    </row>
+    <row r="362" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="2"/>
+      <c r="B362" s="2"/>
+      <c r="C362" s="2"/>
+      <c r="D362" s="2"/>
+    </row>
+    <row r="363" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="2"/>
+      <c r="B363" s="2"/>
+      <c r="C363" s="2"/>
+      <c r="D363" s="2"/>
+    </row>
+    <row r="364" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="2"/>
+      <c r="B364" s="2"/>
+      <c r="C364" s="2"/>
+      <c r="D364" s="2"/>
+    </row>
+    <row r="365" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="2"/>
+      <c r="B365" s="2"/>
+      <c r="C365" s="2"/>
+      <c r="D365" s="2"/>
+    </row>
+    <row r="366" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="2"/>
+      <c r="B366" s="2"/>
+      <c r="C366" s="2"/>
+      <c r="D366" s="2"/>
+    </row>
+    <row r="367" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="2"/>
+      <c r="B367" s="2"/>
+      <c r="C367" s="2"/>
+      <c r="D367" s="2"/>
+    </row>
+    <row r="368" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A368" s="2"/>
+      <c r="B368" s="2"/>
+      <c r="C368" s="2"/>
+      <c r="D368" s="2"/>
+    </row>
+    <row r="369" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A369" s="2"/>
+      <c r="B369" s="2"/>
+      <c r="C369" s="2"/>
+      <c r="D369" s="2"/>
+    </row>
+    <row r="370" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="2"/>
+      <c r="B370" s="2"/>
+      <c r="C370" s="2"/>
+      <c r="D370" s="2"/>
+    </row>
+    <row r="371" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A371" s="2"/>
+      <c r="B371" s="2"/>
+      <c r="C371" s="2"/>
+      <c r="D371" s="2"/>
+    </row>
+    <row r="372" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="2"/>
+      <c r="B372" s="2"/>
+      <c r="C372" s="2"/>
+      <c r="D372" s="2"/>
+    </row>
+    <row r="373" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A373" s="2"/>
+      <c r="B373" s="2"/>
+      <c r="C373" s="2"/>
+      <c r="D373" s="2"/>
+    </row>
+    <row r="374" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="2"/>
+      <c r="B374" s="2"/>
+      <c r="C374" s="2"/>
+      <c r="D374" s="2"/>
+    </row>
+    <row r="375" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A375" s="2"/>
+      <c r="B375" s="2"/>
+      <c r="C375" s="2"/>
+      <c r="D375" s="2"/>
+    </row>
+    <row r="376" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="2"/>
+      <c r="B376" s="2"/>
+      <c r="C376" s="2"/>
+      <c r="D376" s="2"/>
+    </row>
+    <row r="377" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A377" s="2"/>
+      <c r="B377" s="2"/>
+      <c r="C377" s="2"/>
+      <c r="D377" s="2"/>
+    </row>
+    <row r="378" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A378" s="2"/>
+      <c r="B378" s="2"/>
+      <c r="C378" s="2"/>
+      <c r="D378" s="2"/>
+    </row>
+    <row r="379" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A379" s="2"/>
+      <c r="B379" s="2"/>
+      <c r="C379" s="2"/>
+      <c r="D379" s="2"/>
+    </row>
+    <row r="380" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A380" s="2"/>
+      <c r="B380" s="2"/>
+      <c r="C380" s="2"/>
+      <c r="D380" s="2"/>
+    </row>
+    <row r="381" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A381" s="2"/>
+      <c r="B381" s="2"/>
+      <c r="C381" s="2"/>
+      <c r="D381" s="2"/>
+    </row>
+    <row r="382" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A382" s="2"/>
+      <c r="B382" s="2"/>
+      <c r="C382" s="2"/>
+      <c r="D382" s="2"/>
+    </row>
+    <row r="383" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A383" s="2"/>
+      <c r="B383" s="2"/>
+      <c r="C383" s="2"/>
+      <c r="D383" s="2"/>
+    </row>
+    <row r="384" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A384" s="2"/>
+      <c r="B384" s="2"/>
+      <c r="C384" s="2"/>
+      <c r="D384" s="2"/>
+    </row>
+    <row r="385" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A385" s="2"/>
+      <c r="B385" s="2"/>
+      <c r="C385" s="2"/>
+      <c r="D385" s="2"/>
+    </row>
+    <row r="386" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A386" s="2"/>
+      <c r="B386" s="2"/>
+      <c r="C386" s="2"/>
+      <c r="D386" s="2"/>
+    </row>
+    <row r="387" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="2"/>
+      <c r="B387" s="2"/>
+      <c r="C387" s="2"/>
+      <c r="D387" s="2"/>
+    </row>
+    <row r="388" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A388" s="2"/>
+      <c r="B388" s="2"/>
+      <c r="C388" s="2"/>
+      <c r="D388" s="2"/>
+    </row>
+    <row r="389" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A389" s="2"/>
+      <c r="B389" s="2"/>
+      <c r="C389" s="2"/>
+      <c r="D389" s="2"/>
+    </row>
+    <row r="390" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A390" s="2"/>
+      <c r="B390" s="2"/>
+      <c r="C390" s="2"/>
+      <c r="D390" s="2"/>
+    </row>
+    <row r="391" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A391" s="2"/>
+      <c r="B391" s="2"/>
+      <c r="C391" s="2"/>
+      <c r="D391" s="2"/>
+    </row>
+    <row r="392" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A392" s="2"/>
+      <c r="B392" s="2"/>
+      <c r="C392" s="2"/>
+      <c r="D392" s="2"/>
+    </row>
+    <row r="393" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A393" s="2"/>
+      <c r="B393" s="2"/>
+      <c r="C393" s="2"/>
+      <c r="D393" s="2"/>
+    </row>
+    <row r="394" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A394" s="2"/>
+      <c r="B394" s="2"/>
+      <c r="C394" s="2"/>
+      <c r="D394" s="2"/>
+    </row>
+    <row r="395" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A395" s="2"/>
+      <c r="B395" s="2"/>
+      <c r="C395" s="2"/>
+      <c r="D395" s="2"/>
+    </row>
+    <row r="396" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A396" s="2"/>
+      <c r="B396" s="2"/>
+      <c r="C396" s="2"/>
+      <c r="D396" s="2"/>
+    </row>
+    <row r="397" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A397" s="2"/>
+      <c r="B397" s="2"/>
+      <c r="C397" s="2"/>
+      <c r="D397" s="2"/>
+    </row>
+    <row r="398" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A398" s="2"/>
+      <c r="B398" s="2"/>
+      <c r="C398" s="2"/>
+      <c r="D398" s="2"/>
+    </row>
+    <row r="399" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A399" s="2"/>
+      <c r="B399" s="2"/>
+      <c r="C399" s="2"/>
+      <c r="D399" s="2"/>
+    </row>
+    <row r="400" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A400" s="2"/>
+      <c r="B400" s="2"/>
+      <c r="C400" s="2"/>
+      <c r="D400" s="2"/>
+    </row>
+    <row r="401" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A401" s="2"/>
+      <c r="B401" s="2"/>
+      <c r="C401" s="2"/>
+      <c r="D401" s="2"/>
+    </row>
+    <row r="402" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A402" s="2"/>
+      <c r="B402" s="2"/>
+      <c r="C402" s="2"/>
+      <c r="D402" s="2"/>
+    </row>
+    <row r="403" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A403" s="2"/>
+      <c r="B403" s="2"/>
+      <c r="C403" s="2"/>
+      <c r="D403" s="2"/>
+    </row>
+    <row r="404" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A404" s="2"/>
+      <c r="B404" s="2"/>
+      <c r="C404" s="2"/>
+      <c r="D404" s="2"/>
+    </row>
+    <row r="405" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A405" s="2"/>
+      <c r="B405" s="2"/>
+      <c r="C405" s="2"/>
+      <c r="D405" s="2"/>
+    </row>
+    <row r="406" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A406" s="2"/>
+      <c r="B406" s="2"/>
+      <c r="C406" s="2"/>
+      <c r="D406" s="2"/>
+    </row>
+    <row r="407" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A407" s="2"/>
+      <c r="B407" s="2"/>
+      <c r="C407" s="2"/>
+      <c r="D407" s="2"/>
+    </row>
+    <row r="408" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A408" s="2"/>
+      <c r="B408" s="2"/>
+      <c r="C408" s="2"/>
+      <c r="D408" s="2"/>
+    </row>
+    <row r="409" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A409" s="2"/>
+      <c r="B409" s="2"/>
+      <c r="C409" s="2"/>
+      <c r="D409" s="2"/>
+    </row>
+    <row r="410" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A410" s="2"/>
+      <c r="B410" s="2"/>
+      <c r="C410" s="2"/>
+      <c r="D410" s="2"/>
+    </row>
+    <row r="411" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A411" s="2"/>
+      <c r="B411" s="2"/>
+      <c r="C411" s="2"/>
+      <c r="D411" s="2"/>
+    </row>
+    <row r="412" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A412" s="2"/>
+      <c r="B412" s="2"/>
+      <c r="C412" s="2"/>
+      <c r="D412" s="2"/>
+    </row>
+    <row r="413" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A413" s="2"/>
+      <c r="B413" s="2"/>
+      <c r="C413" s="2"/>
+      <c r="D413" s="2"/>
+    </row>
+    <row r="414" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A414" s="2"/>
+      <c r="B414" s="2"/>
+      <c r="C414" s="2"/>
+      <c r="D414" s="2"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>